<commit_message>
correction description placettes (position x y)
</commit_message>
<xml_diff>
--- a/misc/biovimed_teissonniere_2024.xlsx
+++ b/misc/biovimed_teissonniere_2024.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/STAR/02_ACTIONS/ACTION 2/packageR/exemple_data_std/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="190" documentId="11_1B51CE6D7039A9D44BD7707DB2479989811ECAD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F408975-F765-463A-8C76-412ABD47242C}"/>
+  <xr:revisionPtr revIDLastSave="300" documentId="11_1B51CE6D7039A9D44BD7707DB2479989811ECAD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29FA4C1-1DC7-4EBF-8AF2-CCA5A695216A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listes" sheetId="1" state="veryHidden" r:id="rId1"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="144">
   <si>
     <t>suborganization_name</t>
   </si>
@@ -922,6 +922,27 @@
   </si>
   <si>
     <t>D</t>
+  </si>
+  <si>
+    <t>4.475683</t>
+  </si>
+  <si>
+    <t>43.771750</t>
+  </si>
+  <si>
+    <t>Grenache blanc</t>
+  </si>
+  <si>
+    <t>TNT2</t>
+  </si>
+  <si>
+    <t>TNT1</t>
+  </si>
+  <si>
+    <t>TNT3</t>
+  </si>
+  <si>
+    <t>TNT4</t>
   </si>
 </sst>
 </file>
@@ -999,6 +1020,72 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>290451</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>420337</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D29FFB0-CAE4-8742-0A24-FEE79D18C1EC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="5834001" y="304799"/>
+          <a:ext cx="3787486" cy="5400675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -1020,6 +1107,10 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:F45" totalsRowShown="0">
   <autoFilter ref="A1:F45" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F45">
+    <sortCondition ref="D2:D45"/>
+    <sortCondition ref="E2:E45"/>
+  </sortState>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="plot_id" dataDxfId="0">
       <calculatedColumnFormula>CONCATENATE(B2,C2)</calculatedColumnFormula>
@@ -1545,7 +1636,7 @@
   <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K45" sqref="K45"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,6 +1647,9 @@
     <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="16" max="18" width="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="31" width="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1580,14 +1674,14 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
-        <f t="shared" ref="A2:A5" si="0">CONCATENATE(B2,C2)</f>
-        <v>1A</v>
+        <f>CONCATENATE(C2,B2)</f>
+        <v>C2</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1596,205 +1690,204 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="str">
-        <f t="shared" si="0"/>
-        <v>1B</v>
-      </c>
-      <c r="B3">
+      <c r="A3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D3">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
-        <v>134</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
       <c r="E3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>1C</v>
+        <f>CONCATENATE(C4,B4)</f>
+        <v>C5</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>135</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
       <c r="F4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>1D</v>
+        <f>CONCATENATE(C5,B5)</f>
+        <v>C9</v>
       </c>
       <c r="B5">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
-        <v>136</v>
-      </c>
-      <c r="D5">
-        <v>2</v>
-      </c>
       <c r="E5">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="F5">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" ref="A6:A9" si="1">CONCATENATE(B6,C6)</f>
-        <v>2A</v>
+        <f>CONCATENATE(C6,B6)</f>
+        <v>C7</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F6">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="1"/>
-        <v>2B</v>
+        <f>CONCATENATE(C7,B7)</f>
+        <v>C10</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="1"/>
-        <v>2C</v>
+        <f>CONCATENATE(C8,B8)</f>
+        <v>C4</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
         <v>135</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F8">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="1"/>
-        <v>2D</v>
+        <f>CONCATENATE(C9,B9)</f>
+        <v>C8</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F9">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" ref="A10:A13" si="2">CONCATENATE(B10,C10)</f>
-        <v>3A</v>
+        <f>CONCATENATE(C10,B10)</f>
+        <v>C6</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="2"/>
-        <v>3B</v>
+        <f>CONCATENATE(C11,B11)</f>
+        <v>C3</v>
       </c>
       <c r="B11">
         <v>3</v>
       </c>
       <c r="C11" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F11">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="2"/>
-        <v>3C</v>
+        <f>CONCATENATE(C12,B12)</f>
+        <v>C1</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>135</v>
@@ -1803,49 +1896,48 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F12">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="2"/>
-        <v>3D</v>
+        <f>CONCATENATE(C13,B13)</f>
+        <v>D2</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>136</v>
       </c>
       <c r="D13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F13">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="str">
-        <f t="shared" ref="A14:A18" si="3">CONCATENATE(B14,C14)</f>
-        <v>4A</v>
-      </c>
-      <c r="B14">
-        <v>4</v>
+      <c r="A14" t="s">
+        <v>143</v>
+      </c>
+      <c r="B14" t="s">
+        <v>121</v>
       </c>
       <c r="C14" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -1853,53 +1945,53 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="3"/>
-        <v>4B</v>
+        <f>CONCATENATE(C15,B15)</f>
+        <v>D6</v>
       </c>
       <c r="B15">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="F15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="3"/>
-        <v>4C</v>
+        <f>CONCATENATE(C16,B16)</f>
+        <v>D10</v>
       </c>
       <c r="B16">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="F16">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="3"/>
-        <v>4D</v>
+        <f>CONCATENATE(C17,B17)</f>
+        <v>D1</v>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
         <v>136</v>
@@ -1908,238 +2000,237 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F17">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="3"/>
-        <v>5A</v>
+        <f>CONCATENATE(C18,B18)</f>
+        <v>D8</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="F18">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" ref="A19:A45" si="4">CONCATENATE(B19,C19)</f>
-        <v>5B</v>
+        <f>CONCATENATE(C19,B19)</f>
+        <v>D9</v>
       </c>
       <c r="B19">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="F19">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="4"/>
-        <v>5C</v>
+        <f>CONCATENATE(C20,B20)</f>
+        <v>D5</v>
       </c>
       <c r="B20">
         <v>5</v>
       </c>
       <c r="C20" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="F20">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="4"/>
-        <v>5D</v>
+        <f>CONCATENATE(C21,B21)</f>
+        <v>D3</v>
       </c>
       <c r="B21">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>136</v>
       </c>
       <c r="D21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="4"/>
-        <v>6A</v>
+        <f>CONCATENATE(C22,B22)</f>
+        <v>D4</v>
       </c>
       <c r="B22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="F22">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="4"/>
-        <v>6B</v>
+        <f>CONCATENATE(C23,B23)</f>
+        <v>D7</v>
       </c>
       <c r="B23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="F23">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="4"/>
-        <v>6C</v>
+        <f>CONCATENATE(C24,B24)</f>
+        <v>A1</v>
       </c>
       <c r="B24">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E24">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F24">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="4"/>
-        <v>6D</v>
+        <f>CONCATENATE(C25,B25)</f>
+        <v>A8</v>
       </c>
       <c r="B25">
+        <v>8</v>
+      </c>
+      <c r="C25" t="s">
+        <v>133</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
+      <c r="F25">
         <v>6</v>
-      </c>
-      <c r="C25" t="s">
-        <v>136</v>
-      </c>
-      <c r="D25">
-        <v>3</v>
-      </c>
-      <c r="E25">
-        <v>11</v>
-      </c>
-      <c r="F25">
-        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="4"/>
-        <v>7A</v>
+        <f>CONCATENATE(C26,B26)</f>
+        <v>A6</v>
       </c>
       <c r="B26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="s">
         <v>133</v>
       </c>
       <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="E26">
         <v>3</v>
       </c>
-      <c r="E26">
-        <v>2</v>
-      </c>
       <c r="F26">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="4"/>
-        <v>7B</v>
+        <f>CONCATENATE(C27,B27)</f>
+        <v>A3</v>
       </c>
       <c r="B27">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D27">
         <v>2</v>
       </c>
       <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28">
         <v>5</v>
-      </c>
-      <c r="F27">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="str">
-        <f t="shared" si="4"/>
-        <v>7C</v>
-      </c>
-      <c r="B28">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>135</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>8</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -2147,305 +2238,304 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="4"/>
-        <v>7D</v>
+        <f>CONCATENATE(C29,B29)</f>
+        <v>A2</v>
       </c>
       <c r="B29">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E29">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F29">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="4"/>
-        <v>8A</v>
+        <f>CONCATENATE(C30,B30)</f>
+        <v>A9</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C30" t="s">
         <v>133</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="4"/>
-        <v>8B</v>
+        <f>CONCATENATE(C31,B31)</f>
+        <v>A5</v>
       </c>
       <c r="B31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>133</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31">
         <v>8</v>
       </c>
-      <c r="C31" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31">
-        <v>3</v>
-      </c>
-      <c r="E31">
-        <v>5</v>
-      </c>
       <c r="F31">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="4"/>
-        <v>8C</v>
+        <f>CONCATENATE(C32,B32)</f>
+        <v>A7</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D32">
         <v>2</v>
       </c>
       <c r="E32">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F32">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="4"/>
-        <v>8D</v>
+        <f>CONCATENATE(C33,B33)</f>
+        <v>A10</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F33">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="4"/>
-        <v>9A</v>
+        <f>CONCATENATE(C34,B34)</f>
+        <v>A4</v>
       </c>
       <c r="B34">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
         <v>133</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F34">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="4"/>
-        <v>9B</v>
+        <f>CONCATENATE(C35,B35)</f>
+        <v>B5</v>
       </c>
       <c r="B35">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
         <v>134</v>
       </c>
       <c r="D35">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E35">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F35">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="4"/>
-        <v>9C</v>
+        <f>CONCATENATE(C36,B36)</f>
+        <v>B8</v>
       </c>
       <c r="B36">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C36" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F36">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="4"/>
-        <v>9D</v>
+        <f>CONCATENATE(C37,B37)</f>
+        <v>B9</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F37">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="4"/>
-        <v>10A</v>
+        <f>CONCATENATE(C38,B38)</f>
+        <v>B7</v>
       </c>
       <c r="B38">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
       <c r="E38">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="F38">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="4"/>
-        <v>10B</v>
+        <f>CONCATENATE(C39,B39)</f>
+        <v>B3</v>
       </c>
       <c r="B39">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
         <v>134</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F39">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="4"/>
-        <v>10C</v>
+        <f>CONCATENATE(C40,B40)</f>
+        <v>B4</v>
       </c>
       <c r="B40">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E40">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="F40">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="4"/>
-        <v>10D</v>
+        <f>CONCATENATE(C41,B41)</f>
+        <v>B2</v>
       </c>
       <c r="B41">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C41" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E41">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="str">
-        <f t="shared" si="4"/>
-        <v>TNTA</v>
+      <c r="A42" t="s">
+        <v>140</v>
       </c>
       <c r="B42" t="s">
         <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D42">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E42">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="F42">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="4"/>
-        <v>TNTB</v>
-      </c>
-      <c r="B43" t="s">
-        <v>121</v>
+        <f>CONCATENATE(C43,B43)</f>
+        <v>B6</v>
+      </c>
+      <c r="B43">
+        <v>6</v>
       </c>
       <c r="C43" t="s">
         <v>134</v>
@@ -2454,52 +2544,52 @@
         <v>2</v>
       </c>
       <c r="E43">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="F43">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="4"/>
-        <v>TNTC</v>
-      </c>
-      <c r="B44" t="s">
-        <v>121</v>
+        <f>CONCATENATE(C44,B44)</f>
+        <v>B10</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
       </c>
       <c r="C44" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E44">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="F44">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="4"/>
-        <v>TNTD</v>
-      </c>
-      <c r="B45" t="s">
-        <v>121</v>
+        <f>CONCATENATE(C45,B45)</f>
+        <v>B1</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
       </c>
       <c r="C45" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E45">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="F45">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -2511,9 +2601,10 @@
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <legacyDrawing r:id="rId1"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2523,13 +2614,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
@@ -2565,22 +2656,22 @@
         <v>120</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
+        <v>139</v>
+      </c>
+      <c r="C2">
+        <v>2.5</v>
+      </c>
+      <c r="D2">
+        <v>0.9</v>
+      </c>
+      <c r="E2">
+        <v>30034</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>138</v>
       </c>
       <c r="G2" t="s">
-        <v>33</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -2612,7 +2703,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2624,7 +2715,7 @@
     <col min="5" max="5" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2836,9 +2927,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="176" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
mise à jour des fichiers données tests
</commit_message>
<xml_diff>
--- a/misc/biovimed_teissonniere_2024.xlsx
+++ b/misc/biovimed_teissonniere_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vignevin-my.sharepoint.com/personal/xavier_delpuech_vignevin_com/Documents/AgricultureNumerique/ProjetsEnCours/STAR/02_ACTIONS/ACTION 2/packageR/exemple_data_std/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="300" documentId="11_1B51CE6D7039A9D44BD7707DB2479989811ECAD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C29FA4C1-1DC7-4EBF-8AF2-CCA5A695216A}"/>
+  <xr:revisionPtr revIDLastSave="306" documentId="11_1B51CE6D7039A9D44BD7707DB2479989811ECAD0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0D31B9-EB58-401D-9907-0A21C139B679}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32100" yWindow="2490" windowWidth="21600" windowHeight="11235" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="listes" sheetId="1" state="veryHidden" r:id="rId1"/>
@@ -1635,7 +1635,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -1715,7 +1715,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f>CONCATENATE(C4,B4)</f>
+        <f t="shared" ref="A4:A13" si="0">CONCATENATE(C4,B4)</f>
         <v>C5</v>
       </c>
       <c r="B4">
@@ -1736,7 +1736,7 @@
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f>CONCATENATE(C5,B5)</f>
+        <f t="shared" si="0"/>
         <v>C9</v>
       </c>
       <c r="B5">
@@ -1757,7 +1757,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f>CONCATENATE(C6,B6)</f>
+        <f t="shared" si="0"/>
         <v>C7</v>
       </c>
       <c r="B6">
@@ -1778,7 +1778,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f>CONCATENATE(C7,B7)</f>
+        <f t="shared" si="0"/>
         <v>C10</v>
       </c>
       <c r="B7">
@@ -1799,7 +1799,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f>CONCATENATE(C8,B8)</f>
+        <f t="shared" si="0"/>
         <v>C4</v>
       </c>
       <c r="B8">
@@ -1820,7 +1820,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f>CONCATENATE(C9,B9)</f>
+        <f t="shared" si="0"/>
         <v>C8</v>
       </c>
       <c r="B9">
@@ -1841,7 +1841,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f>CONCATENATE(C10,B10)</f>
+        <f t="shared" si="0"/>
         <v>C6</v>
       </c>
       <c r="B10">
@@ -1862,7 +1862,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f>CONCATENATE(C11,B11)</f>
+        <f t="shared" si="0"/>
         <v>C3</v>
       </c>
       <c r="B11">
@@ -1883,7 +1883,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f>CONCATENATE(C12,B12)</f>
+        <f t="shared" si="0"/>
         <v>C1</v>
       </c>
       <c r="B12">
@@ -1904,7 +1904,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f>CONCATENATE(C13,B13)</f>
+        <f t="shared" si="0"/>
         <v>D2</v>
       </c>
       <c r="B13">
@@ -1945,7 +1945,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f>CONCATENATE(C15,B15)</f>
+        <f t="shared" ref="A15:A27" si="1">CONCATENATE(C15,B15)</f>
         <v>D6</v>
       </c>
       <c r="B15">
@@ -1966,7 +1966,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f>CONCATENATE(C16,B16)</f>
+        <f t="shared" si="1"/>
         <v>D10</v>
       </c>
       <c r="B16">
@@ -1987,7 +1987,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f>CONCATENATE(C17,B17)</f>
+        <f t="shared" si="1"/>
         <v>D1</v>
       </c>
       <c r="B17">
@@ -2008,7 +2008,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f>CONCATENATE(C18,B18)</f>
+        <f t="shared" si="1"/>
         <v>D8</v>
       </c>
       <c r="B18">
@@ -2029,7 +2029,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f>CONCATENATE(C19,B19)</f>
+        <f t="shared" si="1"/>
         <v>D9</v>
       </c>
       <c r="B19">
@@ -2050,7 +2050,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f>CONCATENATE(C20,B20)</f>
+        <f t="shared" si="1"/>
         <v>D5</v>
       </c>
       <c r="B20">
@@ -2071,7 +2071,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f>CONCATENATE(C21,B21)</f>
+        <f t="shared" si="1"/>
         <v>D3</v>
       </c>
       <c r="B21">
@@ -2092,7 +2092,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f>CONCATENATE(C22,B22)</f>
+        <f t="shared" si="1"/>
         <v>D4</v>
       </c>
       <c r="B22">
@@ -2113,7 +2113,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f>CONCATENATE(C23,B23)</f>
+        <f t="shared" si="1"/>
         <v>D7</v>
       </c>
       <c r="B23">
@@ -2134,7 +2134,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f>CONCATENATE(C24,B24)</f>
+        <f t="shared" si="1"/>
         <v>A1</v>
       </c>
       <c r="B24">
@@ -2155,7 +2155,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f>CONCATENATE(C25,B25)</f>
+        <f t="shared" si="1"/>
         <v>A8</v>
       </c>
       <c r="B25">
@@ -2176,7 +2176,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f>CONCATENATE(C26,B26)</f>
+        <f t="shared" si="1"/>
         <v>A6</v>
       </c>
       <c r="B26">
@@ -2197,7 +2197,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f>CONCATENATE(C27,B27)</f>
+        <f t="shared" si="1"/>
         <v>A3</v>
       </c>
       <c r="B27">
@@ -2238,7 +2238,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f>CONCATENATE(C29,B29)</f>
+        <f t="shared" ref="A29:A41" si="2">CONCATENATE(C29,B29)</f>
         <v>A2</v>
       </c>
       <c r="B29">
@@ -2259,7 +2259,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f>CONCATENATE(C30,B30)</f>
+        <f t="shared" si="2"/>
         <v>A9</v>
       </c>
       <c r="B30">
@@ -2280,7 +2280,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f>CONCATENATE(C31,B31)</f>
+        <f t="shared" si="2"/>
         <v>A5</v>
       </c>
       <c r="B31">
@@ -2301,7 +2301,7 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f>CONCATENATE(C32,B32)</f>
+        <f t="shared" si="2"/>
         <v>A7</v>
       </c>
       <c r="B32">
@@ -2322,7 +2322,7 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f>CONCATENATE(C33,B33)</f>
+        <f t="shared" si="2"/>
         <v>A10</v>
       </c>
       <c r="B33">
@@ -2343,7 +2343,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f>CONCATENATE(C34,B34)</f>
+        <f t="shared" si="2"/>
         <v>A4</v>
       </c>
       <c r="B34">
@@ -2364,7 +2364,7 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f>CONCATENATE(C35,B35)</f>
+        <f t="shared" si="2"/>
         <v>B5</v>
       </c>
       <c r="B35">
@@ -2385,7 +2385,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f>CONCATENATE(C36,B36)</f>
+        <f t="shared" si="2"/>
         <v>B8</v>
       </c>
       <c r="B36">
@@ -2406,7 +2406,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f>CONCATENATE(C37,B37)</f>
+        <f t="shared" si="2"/>
         <v>B9</v>
       </c>
       <c r="B37">
@@ -2427,7 +2427,7 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f>CONCATENATE(C38,B38)</f>
+        <f t="shared" si="2"/>
         <v>B7</v>
       </c>
       <c r="B38">
@@ -2448,7 +2448,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f>CONCATENATE(C39,B39)</f>
+        <f t="shared" si="2"/>
         <v>B3</v>
       </c>
       <c r="B39">
@@ -2469,7 +2469,7 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f>CONCATENATE(C40,B40)</f>
+        <f t="shared" si="2"/>
         <v>B4</v>
       </c>
       <c r="B40">
@@ -2490,7 +2490,7 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f>CONCATENATE(C41,B41)</f>
+        <f t="shared" si="2"/>
         <v>B2</v>
       </c>
       <c r="B41">
@@ -2927,7 +2927,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>